<commit_message>
updated the layout interpreter and created the traffic_lights_file
</commit_message>
<xml_diff>
--- a/layout/layout_file.xlsx
+++ b/layout/layout_file.xlsx
@@ -582,10 +582,10 @@
   <dimension ref="A1:G4001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D686" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomRight" activeCell="E699" sqref="E699"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated the layout interpreter to read the traffic light information
</commit_message>
<xml_diff>
--- a/layout/layout_file.xlsx
+++ b/layout/layout_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unisabanaedu-my.sharepoint.com/personal/miguelurla_unisabana_edu_co/Documents/GitHub/BRT_C_MEGABUS/layout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="349" documentId="8_{B7FF834D-D2E2-4D46-8DE3-AE5A8C7A8F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{672A6FE9-4625-4ECB-B12E-CE9CB14A1064}"/>
+  <xr:revisionPtr revIDLastSave="350" documentId="8_{B7FF834D-D2E2-4D46-8DE3-AE5A8C7A8F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C5457D5-A583-4084-B914-FBD20064831C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58A8D44C-72FA-46B3-816C-1DB13D289BDA}"/>
   </bookViews>
@@ -582,10 +582,10 @@
   <dimension ref="A1:G4001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D686" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D674" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E699" sqref="E699"/>
+      <selection pane="bottomRight" activeCell="E677" sqref="E677"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7284,7 +7284,7 @@
         <v>25</v>
       </c>
       <c r="E694" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="695" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>